<commit_message>
Data using new search query
</commit_message>
<xml_diff>
--- a/data/PatentSearch/Espacenet/Polymer_countries.xlsx
+++ b/data/PatentSearch/Espacenet/Polymer_countries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Seminar\DataDrivenForesight\data\PatentSearch\Espacenet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DataDrivenForesight\data\PatentSearch\Espacenet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D60528-D38F-44FF-8ED8-03559E1D8F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD57B7E2-07A6-4E72-8FAD-6D6B345BA608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Countries (family)</t>
   </si>
@@ -121,6 +121,84 @@
   </si>
   <si>
     <t>ZA</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>YU</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>UA</t>
   </si>
 </sst>
 </file>
@@ -167,12 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -450,259 +529,467 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1226</v>
+      <c r="B2" s="1">
+        <v>2434</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>100</v>
+      <c r="B3" s="1">
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>95</v>
+      <c r="B4" s="1">
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>75</v>
+      <c r="B5" s="1">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>